<commit_message>
Add a sheet with formula as content in simple_values.xlsx
</commit_message>
<xml_diff>
--- a/sample_excel_files/simple_values.xlsx
+++ b/sample_excel_files/simple_values.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45184DE6-8FCC-E141-B1C9-10A9F1BBEC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98AE692-4C42-2C4B-9CEF-93204F7B088D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
+    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Text</t>
   </si>
@@ -64,6 +65,27 @@
   </si>
   <si>
     <t>Push-ups</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Samosa</t>
+  </si>
+  <si>
+    <t>Satay</t>
+  </si>
+  <si>
+    <t>Nasi Goreng</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -464,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9066D082-A04D-FA4F-B344-A94B465B0F9E}">
   <dimension ref="C4:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -505,4 +527,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add notes and comments to simple_values.xlsx
</commit_message>
<xml_diff>
--- a/sample_excel_files/simple_values.xlsx
+++ b/sample_excel_files/simple_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98AE692-4C42-2C4B-9CEF-93204F7B088D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBD4A70-E6B9-BB49-8ACD-2D3C9DA360F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="15600" activeTab="2" xr2:uid="{E0450653-B2D8-E342-9DE9-A7B7C9F37F08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,71 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D6743592-FF85-FB4F-9157-F70FED5487D6}</author>
+    <author>Ricardo Pramana Suranta</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D6743592-FF85-FB4F-9157-F70FED5487D6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is a sample comment.
+	With tabbed content!
+Another line of comment…
+	With another tabbed comment!</t>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{752A90CA-5197-7E48-ABAA-E663FAE713A7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">This is a sample Note.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">	With tabbed note!
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Another line of note…
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">	With another tabbed comment!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
@@ -92,12 +157,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -138,6 +215,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ricardo Suranta" id="{2F8F8D51-F58F-7A41-A8A4-BACC9E3C6836}" userId="S::rsuranta@andrew.cmu.edu::8fb7d543-eb28-4a0a-9312-b66548c85bb2" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,6 +518,17 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2020-10-16T18:17:01.15" personId="{2F8F8D51-F58F-7A41-A8A4-BACC9E3C6836}" id="{D6743592-FF85-FB4F-9157-F70FED5487D6}">
+    <text>This is a sample comment.
+	With tabbed content!
+Another line of comment…
+	With another tabbed comment!</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7F11B2-676A-8540-BF08-042D2D28BA7D}">
   <dimension ref="A1:B4"/>
@@ -530,11 +624,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C799-78A7-C849-8E49-D29CD30B9485}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,5 +688,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>